<commit_message>
pdfs for full text screen studies file listing full text screenings
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E55CA-77B6-42EB-A9C9-37EB9ED00792}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A71B2B8-9860-4C0B-B1BC-E70FCB9DF867}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$296</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="790">
   <si>
     <t>ID</t>
   </si>
@@ -2366,6 +2369,36 @@
   </si>
   <si>
     <t>review</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>check citations for allocation studies</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>could not download for free</t>
+  </si>
+  <si>
+    <t>need english</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>full text</t>
+  </si>
+  <si>
+    <t>valuable for broad concepts</t>
+  </si>
+  <si>
+    <t>not measurements of interest</t>
+  </si>
+  <si>
+    <t>could not download</t>
   </si>
 </sst>
 </file>
@@ -2691,10 +2724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C273" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G297" sqref="G297"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2730,8 +2764,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2750,6 +2787,9 @@
       <c r="F2" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>772</v>
       </c>
@@ -2757,7 +2797,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2776,11 +2816,14 @@
       <c r="F3" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H3" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2799,11 +2842,14 @@
       <c r="F4" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H4" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2822,11 +2868,14 @@
       <c r="F5" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H5" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2845,11 +2894,14 @@
       <c r="F6" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H6" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2866,10 +2918,16 @@
         <v>2016</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2887,6 +2945,9 @@
       </c>
       <c r="F8" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>776</v>
@@ -2931,8 +2992,9 @@
       <c r="F10" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2951,11 +3013,14 @@
       <c r="F11" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2974,11 +3039,14 @@
       <c r="F12" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2997,11 +3065,14 @@
       <c r="F13" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G13" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3019,6 +3090,9 @@
       </c>
       <c r="F14" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>772</v>
@@ -3064,7 +3138,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3084,7 +3158,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3101,13 +3175,16 @@
         <v>2018</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>775</v>
+        <v>771</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3124,10 +3201,16 @@
         <v>2017</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3146,11 +3229,14 @@
       <c r="F20" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3167,10 +3253,16 @@
         <v>2017</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3189,11 +3281,14 @@
       <c r="F22" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3213,7 +3308,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3230,10 +3325,16 @@
         <v>2016</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3253,7 +3354,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3273,7 +3374,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3292,11 +3393,14 @@
       <c r="F27" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H27" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3316,7 +3420,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3336,7 +3440,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3353,10 +3457,19 @@
         <v>2015</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3373,10 +3486,16 @@
         <v>2015</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3395,11 +3514,14 @@
       <c r="F32" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G32" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H32" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3418,11 +3540,14 @@
       <c r="F33" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H33" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3439,10 +3564,16 @@
         <v>2018</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3461,11 +3592,14 @@
       <c r="F35" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H35" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3484,11 +3618,14 @@
       <c r="F36" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G36" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H36" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3507,11 +3644,14 @@
       <c r="F37" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G37" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H37" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3528,10 +3668,16 @@
         <v>2018</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3548,10 +3694,16 @@
         <v>2018</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3570,11 +3722,14 @@
       <c r="F40" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G40" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H40" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3593,11 +3748,14 @@
       <c r="F41" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G41" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H41" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3617,7 +3775,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3637,7 +3795,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3657,7 +3815,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3676,11 +3834,14 @@
       <c r="F45" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G45" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H45" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3697,10 +3858,16 @@
         <v>2017</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3719,8 +3886,11 @@
       <c r="F47" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3740,7 +3910,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3760,7 +3930,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3779,11 +3949,14 @@
       <c r="F50" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H50" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3802,11 +3975,14 @@
       <c r="F51" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H51" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3826,7 +4002,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3845,11 +4021,14 @@
       <c r="F53" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G53" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H53" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3868,11 +4047,14 @@
       <c r="F54" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G54" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H54" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3892,7 +4074,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3911,11 +4093,14 @@
       <c r="F56" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G56" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H56" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3934,11 +4119,14 @@
       <c r="F57" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G57" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H57" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3957,11 +4145,14 @@
       <c r="F58" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G58" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H58" s="2" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3978,10 +4169,16 @@
         <v>2015</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3998,10 +4195,19 @@
         <v>2015</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4018,10 +4224,19 @@
         <v>2015</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4038,10 +4253,19 @@
         <v>2015</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4060,8 +4284,11 @@
       <c r="F63" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4080,11 +4307,14 @@
       <c r="F64" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G64" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H64" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4102,6 +4332,9 @@
       </c>
       <c r="F65" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>772</v>
@@ -4127,7 +4360,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4146,11 +4379,14 @@
       <c r="F67" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G67" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H67" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4169,11 +4405,14 @@
       <c r="F68" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H68" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4192,11 +4431,14 @@
       <c r="F69" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G69" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H69" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4215,11 +4457,14 @@
       <c r="F70" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H70" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4237,6 +4482,9 @@
       </c>
       <c r="F71" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>776</v>
@@ -4262,7 +4510,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4281,11 +4529,14 @@
       <c r="F73" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G73" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H73" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4304,11 +4555,14 @@
       <c r="F74" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G74" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H74" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4327,11 +4581,14 @@
       <c r="F75" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G75" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H75" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4350,11 +4607,14 @@
       <c r="F76" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G76" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H76" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4373,11 +4633,14 @@
       <c r="F77" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G77" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H77" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4395,6 +4658,9 @@
       </c>
       <c r="F78" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>772</v>
@@ -4440,7 +4706,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4459,11 +4725,14 @@
       <c r="F81" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G81" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H81" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4480,10 +4749,16 @@
         <v>2018</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4502,11 +4777,14 @@
       <c r="F83" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G83" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H83" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4525,11 +4803,14 @@
       <c r="F84" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H84" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4548,11 +4829,14 @@
       <c r="F85" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G85" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H85" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4571,11 +4855,14 @@
       <c r="F86" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G86" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H86" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4594,11 +4881,14 @@
       <c r="F87" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G87" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H87" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4617,11 +4907,14 @@
       <c r="F88" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H88" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4640,11 +4933,14 @@
       <c r="F89" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G89" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H89" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4663,11 +4959,14 @@
       <c r="F90" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G90" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H90" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4684,10 +4983,19 @@
         <v>2015</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4704,10 +5012,16 @@
         <v>2014</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4726,11 +5040,14 @@
       <c r="F93" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H93" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4749,11 +5066,14 @@
       <c r="F94" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H94" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4772,11 +5092,14 @@
       <c r="F95" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H95" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4795,11 +5118,14 @@
       <c r="F96" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H96" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4816,10 +5142,16 @@
         <v>2016</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4836,10 +5168,16 @@
         <v>2015</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4858,11 +5196,14 @@
       <c r="F99" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G99" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H99" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4881,11 +5222,14 @@
       <c r="F100" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G100" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H100" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4904,11 +5248,14 @@
       <c r="F101" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G101" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H101" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4927,11 +5274,14 @@
       <c r="F102" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G102" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H102" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4950,11 +5300,14 @@
       <c r="F103" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G103" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H103" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4973,11 +5326,14 @@
       <c r="F104" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G104" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H104" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4994,10 +5350,16 @@
         <v>2015</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5016,11 +5378,14 @@
       <c r="F106" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G106" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H106" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5039,11 +5404,14 @@
       <c r="F107" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G107" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H107" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5060,10 +5428,16 @@
         <v>2016</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5080,10 +5454,16 @@
         <v>2015</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5102,11 +5482,14 @@
       <c r="F110" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G110" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H110" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5123,10 +5506,16 @@
         <v>2016</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5145,11 +5534,14 @@
       <c r="F112" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G112" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H112" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5168,11 +5560,14 @@
       <c r="F113" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G113" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H113" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5191,11 +5586,14 @@
       <c r="F114" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G114" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H114" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5212,10 +5610,16 @@
         <v>2014</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5232,10 +5636,16 @@
         <v>2014</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5254,11 +5664,14 @@
       <c r="F117" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H117" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5275,10 +5688,16 @@
         <v>2014</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5297,11 +5716,14 @@
       <c r="F119" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G119" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H119" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5318,10 +5740,16 @@
         <v>2016</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5340,11 +5768,14 @@
       <c r="F121" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G121" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H121" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5363,11 +5794,14 @@
       <c r="F122" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G122" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H122" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5386,11 +5820,14 @@
       <c r="F123" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G123" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H123" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5409,11 +5846,14 @@
       <c r="F124" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H124" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5432,11 +5872,14 @@
       <c r="F125" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H125" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5455,11 +5898,14 @@
       <c r="F126" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H126" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5478,11 +5924,14 @@
       <c r="F127" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G127" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H127" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5499,10 +5948,19 @@
         <v>2016</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="I128" s="2" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5521,11 +5979,14 @@
       <c r="F129" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G129" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H129" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5544,11 +6005,14 @@
       <c r="F130" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G130" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H130" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5567,11 +6031,14 @@
       <c r="F131" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H131" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5590,11 +6057,14 @@
       <c r="F132" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G132" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H132" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5613,11 +6083,14 @@
       <c r="F133" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G133" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H133" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5636,11 +6109,14 @@
       <c r="F134" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G134" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H134" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5657,10 +6133,16 @@
         <v>2014</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5679,11 +6161,14 @@
       <c r="F136" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G136" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H136" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5702,11 +6187,14 @@
       <c r="F137" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G137" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H137" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5725,11 +6213,14 @@
       <c r="F138" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H138" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5746,10 +6237,16 @@
         <v>2018</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5768,11 +6265,14 @@
       <c r="F140" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H140" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5791,11 +6291,14 @@
       <c r="F141" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G141" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H141" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5812,10 +6315,16 @@
         <v>2018</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5832,13 +6341,16 @@
         <v>2018</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>775</v>
+        <v>771</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5857,11 +6369,14 @@
       <c r="F144" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G144" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H144" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5880,11 +6395,14 @@
       <c r="F145" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G145" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H145" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5901,10 +6419,16 @@
         <v>2018</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5923,11 +6447,14 @@
       <c r="F147" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G147" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H147" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5944,10 +6471,16 @@
         <v>2017</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5966,11 +6499,14 @@
       <c r="F149" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G149" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H149" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5989,11 +6525,14 @@
       <c r="F150" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G150" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H150" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6012,11 +6551,14 @@
       <c r="F151" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G151" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H151" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6033,10 +6575,16 @@
         <v>2017</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6055,11 +6603,14 @@
       <c r="F153" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G153" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H153" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6076,10 +6627,16 @@
         <v>2016</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6098,11 +6655,14 @@
       <c r="F155" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G155" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H155" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6119,10 +6679,16 @@
         <v>2015</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6139,10 +6705,16 @@
         <v>2014</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G157" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6161,11 +6733,14 @@
       <c r="F158" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G158" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H158" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6184,11 +6759,14 @@
       <c r="F159" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G159" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H159" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6207,11 +6785,14 @@
       <c r="F160" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G160" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H160" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6230,11 +6811,14 @@
       <c r="F161" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G161" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H161" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6252,6 +6836,9 @@
       </c>
       <c r="F162" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G162" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H162" s="2" t="s">
         <v>776</v>
@@ -6277,7 +6864,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6294,10 +6881,16 @@
         <v>2015</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G164" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6316,11 +6909,14 @@
       <c r="F165" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G165" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H165" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6338,6 +6934,9 @@
       </c>
       <c r="F166" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G166" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H166" s="2" t="s">
         <v>773</v>
@@ -6363,7 +6962,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6382,11 +6981,14 @@
       <c r="F168" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G168" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H168" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6405,11 +7007,14 @@
       <c r="F169" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G169" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H169" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6428,11 +7033,14 @@
       <c r="F170" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G170" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H170" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6449,10 +7057,16 @@
         <v>2015</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6471,11 +7085,14 @@
       <c r="F172" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G172" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H172" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6494,11 +7111,14 @@
       <c r="F173" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G173" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H173" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6517,11 +7137,14 @@
       <c r="F174" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G174" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H174" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6540,11 +7163,14 @@
       <c r="F175" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G175" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H175" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6563,11 +7189,14 @@
       <c r="F176" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G176" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H176" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6586,11 +7215,14 @@
       <c r="F177" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G177" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H177" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6609,11 +7241,14 @@
       <c r="F178" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G178" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H178" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6632,11 +7267,14 @@
       <c r="F179" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G179" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H179" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6653,10 +7291,16 @@
         <v>2015</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6675,11 +7319,14 @@
       <c r="F181" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G181" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H181" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6697,6 +7344,9 @@
       </c>
       <c r="F182" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G182" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H182" s="2" t="s">
         <v>772</v>
@@ -6722,7 +7372,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6741,11 +7391,14 @@
       <c r="F184" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G184" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H184" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6764,11 +7417,14 @@
       <c r="F185" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G185" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H185" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6787,11 +7443,14 @@
       <c r="F186" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G186" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H186" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6810,11 +7469,14 @@
       <c r="F187" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G187" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H187" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6833,11 +7495,14 @@
       <c r="F188" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G188" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H188" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6856,11 +7521,14 @@
       <c r="F189" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G189" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H189" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6879,11 +7547,14 @@
       <c r="F190" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G190" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H190" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6900,10 +7571,16 @@
         <v>2017</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6920,10 +7597,16 @@
         <v>2017</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G192" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6942,11 +7625,14 @@
       <c r="F193" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G193" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H193" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6965,11 +7651,14 @@
       <c r="F194" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G194" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H194" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6986,7 +7675,13 @@
         <v>2016</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>775</v>
+        <v>771</v>
+      </c>
+      <c r="G195" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
@@ -7009,7 +7704,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>196</v>
       </c>
@@ -7028,11 +7723,14 @@
       <c r="F197" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G197" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H197" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>197</v>
       </c>
@@ -7051,11 +7749,14 @@
       <c r="F198" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G198" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H198" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>198</v>
       </c>
@@ -7074,11 +7775,14 @@
       <c r="F199" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G199" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H199" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>199</v>
       </c>
@@ -7097,11 +7801,14 @@
       <c r="F200" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G200" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H200" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7120,11 +7827,14 @@
       <c r="F201" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G201" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H201" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>201</v>
       </c>
@@ -7143,11 +7853,14 @@
       <c r="F202" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G202" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H202" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>202</v>
       </c>
@@ -7166,11 +7879,14 @@
       <c r="F203" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G203" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H203" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>203</v>
       </c>
@@ -7189,11 +7905,14 @@
       <c r="F204" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G204" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H204" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>204</v>
       </c>
@@ -7212,11 +7931,14 @@
       <c r="F205" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G205" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H205" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>205</v>
       </c>
@@ -7235,11 +7957,14 @@
       <c r="F206" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G206" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H206" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>206</v>
       </c>
@@ -7258,11 +7983,14 @@
       <c r="F207" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G207" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H207" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>207</v>
       </c>
@@ -7281,11 +8009,14 @@
       <c r="F208" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G208" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H208" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>208</v>
       </c>
@@ -7304,11 +8035,14 @@
       <c r="F209" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G209" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H209" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7327,11 +8061,14 @@
       <c r="F210" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G210" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H210" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7348,10 +8085,16 @@
         <v>2018</v>
       </c>
       <c r="F211" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7370,11 +8113,14 @@
       <c r="F212" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G212" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H212" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7393,11 +8139,14 @@
       <c r="F213" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G213" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H213" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7416,11 +8165,14 @@
       <c r="F214" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G214" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H214" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>214</v>
       </c>
@@ -7439,11 +8191,14 @@
       <c r="F215" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G215" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H215" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>215</v>
       </c>
@@ -7462,11 +8217,14 @@
       <c r="F216" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G216" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H216" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>216</v>
       </c>
@@ -7485,8 +8243,11 @@
       <c r="F217" s="2" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I217" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>217</v>
       </c>
@@ -7505,11 +8266,14 @@
       <c r="F218" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G218" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H218" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>218</v>
       </c>
@@ -7528,11 +8292,14 @@
       <c r="F219" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G219" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H219" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>219</v>
       </c>
@@ -7551,11 +8318,14 @@
       <c r="F220" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G220" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H220" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>220</v>
       </c>
@@ -7574,11 +8344,14 @@
       <c r="F221" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G221" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H221" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>221</v>
       </c>
@@ -7597,11 +8370,14 @@
       <c r="F222" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G222" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H222" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>222</v>
       </c>
@@ -7618,10 +8394,19 @@
         <v>2018</v>
       </c>
       <c r="F223" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G223" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H223" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I223" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>223</v>
       </c>
@@ -7640,11 +8425,14 @@
       <c r="F224" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G224" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H224" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>224</v>
       </c>
@@ -7662,6 +8450,9 @@
       </c>
       <c r="F225" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G225" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H225" s="2" t="s">
         <v>772</v>
@@ -7687,7 +8478,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>226</v>
       </c>
@@ -7706,11 +8497,14 @@
       <c r="F227" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G227" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H227" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>227</v>
       </c>
@@ -7727,10 +8521,16 @@
         <v>2017</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G228" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H228" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>228</v>
       </c>
@@ -7748,6 +8548,9 @@
       </c>
       <c r="F229" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G229" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H229" s="2" t="s">
         <v>773</v>
@@ -7773,7 +8576,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>230</v>
       </c>
@@ -7791,6 +8594,9 @@
       </c>
       <c r="F231" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G231" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H231" s="2" t="s">
         <v>773</v>
@@ -7836,7 +8642,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>233</v>
       </c>
@@ -7855,11 +8661,14 @@
       <c r="F234" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G234" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H234" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>234</v>
       </c>
@@ -7878,11 +8687,14 @@
       <c r="F235" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G235" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H235" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>235</v>
       </c>
@@ -7901,11 +8713,14 @@
       <c r="F236" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G236" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H236" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>236</v>
       </c>
@@ -7924,11 +8739,14 @@
       <c r="F237" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G237" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H237" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>237</v>
       </c>
@@ -7947,11 +8765,14 @@
       <c r="F238" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G238" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H238" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>238</v>
       </c>
@@ -7968,10 +8789,16 @@
         <v>2016</v>
       </c>
       <c r="F239" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G239" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>239</v>
       </c>
@@ -7990,11 +8817,14 @@
       <c r="F240" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G240" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H240" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>240</v>
       </c>
@@ -8014,7 +8844,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>241</v>
       </c>
@@ -8031,10 +8861,16 @@
         <v>2016</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G242" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>242</v>
       </c>
@@ -8053,11 +8889,14 @@
       <c r="F243" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G243" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H243" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>243</v>
       </c>
@@ -8074,10 +8913,19 @@
         <v>2015</v>
       </c>
       <c r="F244" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G244" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I244" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>244</v>
       </c>
@@ -8096,11 +8944,14 @@
       <c r="F245" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G245" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H245" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>245</v>
       </c>
@@ -8117,11 +8968,16 @@
         <v>2015</v>
       </c>
       <c r="F246" s="2" t="s">
-        <v>775</v>
-      </c>
-      <c r="H246" s="2"/>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G246" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>246</v>
       </c>
@@ -8140,11 +8996,14 @@
       <c r="F247" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G247" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H247" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>247</v>
       </c>
@@ -8163,11 +9022,14 @@
       <c r="F248" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G248" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H248" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>248</v>
       </c>
@@ -8186,11 +9048,14 @@
       <c r="F249" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G249" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H249" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>249</v>
       </c>
@@ -8209,11 +9074,14 @@
       <c r="F250" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G250" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H250" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>250</v>
       </c>
@@ -8232,11 +9100,14 @@
       <c r="F251" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G251" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H251" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>251</v>
       </c>
@@ -8256,7 +9127,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>252</v>
       </c>
@@ -8276,7 +9147,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>253</v>
       </c>
@@ -8296,7 +9167,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>254</v>
       </c>
@@ -8313,10 +9184,19 @@
         <v>2015</v>
       </c>
       <c r="F255" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G255" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H255" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="I255" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>255</v>
       </c>
@@ -8335,11 +9215,14 @@
       <c r="F256" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G256" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H256" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>256</v>
       </c>
@@ -8358,11 +9241,14 @@
       <c r="F257" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G257" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H257" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>257</v>
       </c>
@@ -8379,10 +9265,16 @@
         <v>2014</v>
       </c>
       <c r="F258" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G258" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H258" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>258</v>
       </c>
@@ -8401,11 +9293,14 @@
       <c r="F259" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G259" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H259" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>259</v>
       </c>
@@ -8424,11 +9319,14 @@
       <c r="F260" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G260" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H260" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>260</v>
       </c>
@@ -8447,11 +9345,14 @@
       <c r="F261" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G261" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H261" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>261</v>
       </c>
@@ -8470,11 +9371,14 @@
       <c r="F262" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G262" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H262" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>262</v>
       </c>
@@ -8493,11 +9397,14 @@
       <c r="F263" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G263" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H263" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>263</v>
       </c>
@@ -8516,11 +9423,14 @@
       <c r="F264" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G264" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H264" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>264</v>
       </c>
@@ -8539,11 +9449,14 @@
       <c r="F265" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G265" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H265" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>265</v>
       </c>
@@ -8562,11 +9475,14 @@
       <c r="F266" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G266" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H266" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>266</v>
       </c>
@@ -8585,11 +9501,14 @@
       <c r="F267" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G267" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H267" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>267</v>
       </c>
@@ -8606,10 +9525,16 @@
         <v>2017</v>
       </c>
       <c r="F268" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G268" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H268" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>268</v>
       </c>
@@ -8628,11 +9553,14 @@
       <c r="F269" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G269" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H269" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>269</v>
       </c>
@@ -8651,11 +9579,14 @@
       <c r="F270" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G270" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H270" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>270</v>
       </c>
@@ -8674,11 +9605,14 @@
       <c r="F271" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G271" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H271" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>271</v>
       </c>
@@ -8697,11 +9631,14 @@
       <c r="F272" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G272" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H272" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>272</v>
       </c>
@@ -8720,11 +9657,14 @@
       <c r="F273" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G273" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H273" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>273</v>
       </c>
@@ -8743,11 +9683,14 @@
       <c r="F274" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G274" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H274" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>274</v>
       </c>
@@ -8766,11 +9709,14 @@
       <c r="F275" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G275" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H275" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>275</v>
       </c>
@@ -8789,11 +9735,14 @@
       <c r="F276" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G276" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H276" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>276</v>
       </c>
@@ -8810,10 +9759,16 @@
         <v>2017</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G277" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H277" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>277</v>
       </c>
@@ -8832,11 +9787,14 @@
       <c r="F278" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G278" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H278" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>278</v>
       </c>
@@ -8855,11 +9813,14 @@
       <c r="F279" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G279" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H279" s="2" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>279</v>
       </c>
@@ -8876,11 +9837,16 @@
         <v>2016</v>
       </c>
       <c r="F280" s="2" t="s">
-        <v>775</v>
-      </c>
-      <c r="H280" s="2"/>
-    </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+        <v>771</v>
+      </c>
+      <c r="G280" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H280" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>280</v>
       </c>
@@ -8899,11 +9865,14 @@
       <c r="F281" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G281" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H281" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>281</v>
       </c>
@@ -8919,11 +9888,17 @@
       <c r="E282">
         <v>2016</v>
       </c>
+      <c r="F282" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="G282" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H282" s="2" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>282</v>
       </c>
@@ -8942,11 +9917,14 @@
       <c r="F283" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G283" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H283" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>283</v>
       </c>
@@ -8965,11 +9943,14 @@
       <c r="F284" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G284" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H284" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>284</v>
       </c>
@@ -8988,11 +9969,14 @@
       <c r="F285" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G285" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H285" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>285</v>
       </c>
@@ -9010,6 +9994,9 @@
       </c>
       <c r="F286" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G286" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H286" s="2" t="s">
         <v>772</v>
@@ -9035,7 +10022,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>287</v>
       </c>
@@ -9054,11 +10041,14 @@
       <c r="F288" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G288" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H288" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>288</v>
       </c>
@@ -9077,11 +10067,14 @@
       <c r="F289" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G289" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H289" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>289</v>
       </c>
@@ -9100,11 +10093,14 @@
       <c r="F290" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G290" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H290" s="2" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>290</v>
       </c>
@@ -9123,11 +10119,14 @@
       <c r="F291" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G291" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H291" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>291</v>
       </c>
@@ -9145,6 +10144,9 @@
       </c>
       <c r="F292" s="2" t="s">
         <v>771</v>
+      </c>
+      <c r="G292" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H292" s="2" t="s">
         <v>772</v>
@@ -9170,7 +10172,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>293</v>
       </c>
@@ -9189,11 +10191,14 @@
       <c r="F294" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G294" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H294" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>294</v>
       </c>
@@ -9212,11 +10217,14 @@
       <c r="F295" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G295" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H295" s="2" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>295</v>
       </c>
@@ -9235,11 +10243,21 @@
       <c r="F296" s="2" t="s">
         <v>771</v>
       </c>
+      <c r="G296" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H296" s="2" t="s">
         <v>776</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I296" xr:uid="{689CF9D2-75D4-40E0-9527-98FA83F8B958}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>